<commit_message>
First batch of basic localization test working
</commit_message>
<xml_diff>
--- a/test/loc_All objects_fr.xlsx
+++ b/test/loc_All objects_fr.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Project\articy-node\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB35F931-61A1-4348-8D42-69D986BFA9F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B09A411-4C43-445A-926E-67001F04B3CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ArticyStrings" sheetId="2" r:id="rId1"/>
@@ -229,9 +229,6 @@
     <t>FFr_10EB377E.DisplayName</t>
   </si>
   <si>
-    <t>Text Node</t>
-  </si>
-  <si>
     <t>Flow/Text Node</t>
   </si>
   <si>
@@ -284,6 +281,9 @@
   </si>
   <si>
     <t>This is some French text.</t>
+  </si>
+  <si>
+    <t>French Node</t>
   </si>
 </sst>
 </file>
@@ -644,8 +644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -939,82 +939,82 @@
         <v>68</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>70</v>
       </c>
       <c r="D24" s="2"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D25" s="2"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>74</v>
       </c>
       <c r="D26" s="2"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>77</v>
       </c>
       <c r="D27" s="2"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>80</v>
       </c>
       <c r="D28" s="2"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>83</v>
       </c>
       <c r="D29" s="2"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="D30" s="2"/>
     </row>

</xml_diff>